<commit_message>
add BOM mini6ch v1.2
</commit_message>
<xml_diff>
--- a/Mazduino-Mini-6CH/v1.2/BOM.xlsx
+++ b/Mazduino-Mini-6CH/v1.2/BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amri/DIY_ECU/Mazduino/Mazduino-Mini-6CH/v1.2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8830D038-ECD6-9440-937E-9BE3E1163887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F8AC87-E1B7-9745-9088-F08C2CEBD586}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16000" xr2:uid="{78526EDA-D430-D94A-9015-2067DB7682F6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26740" xr2:uid="{78526EDA-D430-D94A-9015-2067DB7682F6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{3028AAF8-B511-D048-AA38-0338EB9A54CF}" name="mazduino_base" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/amri/DIY_ECU/Speeduino/MAZDUNO ECU/Mini_6ch/Mazduino_mini_6CH_v1.2/mazduino_base.csv" decimal="," thousands="." tab="0" comma="1">
+    <textPr sourceFile="/Users/amri/DIY_ECU/Speeduino/MAZDUNO ECU/Mini_6ch/Mazduino_mini_6CH_v1.2/mazduino_base.csv" decimal="," thousands="." tab="0" comma="1">
       <textFields count="4">
         <textField/>
         <textField/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="161">
   <si>
     <t>Reference</t>
   </si>
@@ -248,9 +248,6 @@
     <t>J9</t>
   </si>
   <si>
-    <t>S48B-ZROK-2A-R</t>
-  </si>
-  <si>
     <t>S48BZROK2AR</t>
   </si>
   <si>
@@ -305,9 +302,6 @@
     <t>Q1,Q2,Q3,Q4,Q6,Q10,Q11,Q12</t>
   </si>
   <si>
-    <t>Q_NMOS_GDS</t>
-  </si>
-  <si>
     <t>Package_TO_SOT_SMD:SOT-223-3_TabPin2</t>
   </si>
   <si>
@@ -395,9 +389,6 @@
     <t>R52,R53,R54,R55,R105,R106</t>
   </si>
   <si>
-    <t>15R</t>
-  </si>
-  <si>
     <t>Resistor_SMD:R_2512_6332Metric</t>
   </si>
   <si>
@@ -537,6 +528,15 @@
   </si>
   <si>
     <t>Crystal:Crystal_SMD_3215-2Pin_3.2x1.5mm</t>
+  </si>
+  <si>
+    <t>Yamaha 48p</t>
+  </si>
+  <si>
+    <t>15R 2W</t>
+  </si>
+  <si>
+    <t>BSP78/NCV8405A/NCV8406A</t>
   </si>
 </sst>
 </file>
@@ -941,14 +941,14 @@
   </sheetPr>
   <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
       <selection sqref="A1:D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="47" customWidth="1"/>
-    <col min="2" max="2" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4" bestFit="1" customWidth="1"/>
   </cols>
@@ -1237,8 +1237,8 @@
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="2">
-        <v>1206</v>
+      <c r="B21" s="2" t="s">
+        <v>48</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>49</v>
@@ -1308,10 +1308,10 @@
         <v>63</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>65</v>
       </c>
       <c r="D26" s="2">
         <v>1</v>
@@ -1319,13 +1319,13 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D27" s="2">
         <v>1</v>
@@ -1333,13 +1333,13 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>70</v>
-      </c>
       <c r="C28" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D28" s="2">
         <v>2</v>
@@ -1347,13 +1347,13 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="D29" s="2">
         <v>2</v>
@@ -1361,10 +1361,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>74</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>32</v>
@@ -1375,13 +1375,13 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="D31" s="2">
         <v>1</v>
@@ -1389,13 +1389,13 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="D32" s="2">
         <v>1</v>
@@ -1403,13 +1403,13 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="D33" s="2">
         <v>8</v>
@@ -1417,10 +1417,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>46</v>
@@ -1431,10 +1431,10 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>46</v>
@@ -1445,13 +1445,13 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="D36" s="2">
         <v>8</v>
@@ -1459,13 +1459,13 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D37" s="2">
         <v>19</v>
@@ -1473,13 +1473,13 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D38" s="2">
         <v>14</v>
@@ -1487,13 +1487,13 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D39" s="2">
         <v>6</v>
@@ -1501,13 +1501,13 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D40" s="2">
         <v>6</v>
@@ -1515,13 +1515,13 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D41" s="2">
         <v>26</v>
@@ -1529,13 +1529,13 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D42" s="2">
         <v>9</v>
@@ -1543,13 +1543,13 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D43" s="2">
         <v>1</v>
@@ -1557,13 +1557,13 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D44" s="2">
         <v>2</v>
@@ -1571,13 +1571,13 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D45" s="2">
         <v>5</v>
@@ -1585,13 +1585,13 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D46" s="2">
         <v>3</v>
@@ -1599,13 +1599,13 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>113</v>
+        <v>159</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D47" s="2">
         <v>6</v>
@@ -1613,13 +1613,13 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D48" s="2">
         <v>3</v>
@@ -1627,13 +1627,13 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D49" s="2">
         <v>1</v>
@@ -1641,13 +1641,13 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D50" s="2">
         <v>2</v>
@@ -1655,13 +1655,13 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D51" s="2">
         <v>3</v>
@@ -1669,13 +1669,13 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D52" s="2">
         <v>1</v>
@@ -1683,13 +1683,13 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D53" s="2">
         <v>2</v>
@@ -1697,13 +1697,13 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D54" s="2">
         <v>1</v>
@@ -1711,13 +1711,13 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D55" s="2">
         <v>2</v>
@@ -1725,13 +1725,13 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D56" s="2">
         <v>2</v>
@@ -1739,13 +1739,13 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D57" s="2">
         <v>1</v>
@@ -1753,13 +1753,13 @@
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D58" s="2">
         <v>3</v>
@@ -1767,13 +1767,13 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D59" s="2">
         <v>1</v>
@@ -1781,13 +1781,13 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D60" s="2">
         <v>2</v>
@@ -1795,13 +1795,13 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D61" s="2">
         <v>1</v>
@@ -1809,13 +1809,13 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="D62" s="2">
         <v>1</v>
@@ -1823,13 +1823,13 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D63" s="2">
         <v>1</v>
@@ -1837,13 +1837,13 @@
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="D64" s="2">
         <v>1</v>
@@ -1851,13 +1851,13 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D65" s="2">
         <v>1</v>

</xml_diff>